<commit_message>
Removed extraneous notes from spreadsheet
</commit_message>
<xml_diff>
--- a/BESTFiles/Gatekeeper - Scoresheet.xlsx
+++ b/BESTFiles/Gatekeeper - Scoresheet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="76">
   <si>
     <t>AND</t>
   </si>
@@ -227,6 +227,24 @@
   </si>
   <si>
     <t>Dlatch</t>
+  </si>
+  <si>
+    <t>5S</t>
+  </si>
+  <si>
+    <t>5S %</t>
+  </si>
+  <si>
+    <t>5S max</t>
+  </si>
+  <si>
+    <t>5S earned</t>
+  </si>
+  <si>
+    <t>Final Total</t>
+  </si>
+  <si>
+    <t>DQ</t>
   </si>
 </sst>
 </file>
@@ -465,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -668,6 +686,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1189,10 +1211,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CA81"/>
+  <dimension ref="A1:CC81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="CC3" sqref="CC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,8 +1247,10 @@
     <col min="80" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A1" s="37"/>
+    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>75</v>
+      </c>
       <c r="B1" s="37"/>
       <c r="C1" s="52" t="s">
         <v>20</v>
@@ -1271,11 +1295,23 @@
       </c>
       <c r="AN1" s="53"/>
       <c r="AO1" s="53"/>
+      <c r="AP1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ1" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="AS1" s="9" t="s">
         <v>37</v>
       </c>
+      <c r="CB1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="CC1" s="9" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="72" t="s">
@@ -1345,9 +1381,16 @@
       <c r="AM2" s="33"/>
       <c r="AN2" s="38">
         <f>$AP8+$AP18+$AP28+$AP38+$AP48+$AP58+$AP68+$AP78</f>
-        <v>0</v>
+        <v>4224</v>
       </c>
       <c r="AO2" s="8"/>
+      <c r="AP2" s="9">
+        <f>(SUMIF('Conversion Cheatsheet'!AD2:AD9,"=0",'Conversion Cheatsheet'!AC2:AC9)/COUNTIF('Conversion Cheatsheet'!AD2:AD9,"=0"))</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AQ2" s="81">
+        <v>0.1</v>
+      </c>
       <c r="AS2" s="41" t="s">
         <v>4</v>
       </c>
@@ -1413,8 +1456,16 @@
       <c r="BY2" s="41"/>
       <c r="BZ2" s="41"/>
       <c r="CA2" s="41"/>
+      <c r="CB2" s="9">
+        <f>AP2*AQ2</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="CC2" s="9">
+        <f>AN2*(1+CB2)</f>
+        <v>4505.6000000000004</v>
+      </c>
     </row>
-    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="12" t="s">
@@ -1618,7 +1669,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A4" s="62">
         <v>1</v>
       </c>
@@ -1763,7 +1814,7 @@
       <c r="BZ4" s="41"/>
       <c r="CA4" s="41"/>
     </row>
-    <row r="5" spans="1:79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="14" t="s">
         <v>6</v>
@@ -1775,7 +1826,9 @@
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
       <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
+      <c r="J5" s="31">
+        <v>20</v>
+      </c>
       <c r="K5" s="30"/>
       <c r="L5" s="65"/>
       <c r="M5" s="67"/>
@@ -1824,7 +1877,7 @@
       </c>
       <c r="AV5" s="16">
         <f>$I7</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="AW5" s="16">
         <f>$C7-$AS7</f>
@@ -1840,7 +1893,7 @@
       </c>
       <c r="AZ5" s="16">
         <f>$I7-$AV7</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="BA5" s="16">
         <f>$C7-$AS7-$AW7</f>
@@ -1856,7 +1909,7 @@
       </c>
       <c r="BD5" s="16">
         <f>$I7-$AV7-$AZ7</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="BE5" s="16">
         <f>$C7-$AS7-$AW7-$BA7</f>
@@ -1872,7 +1925,7 @@
       </c>
       <c r="BH5" s="16">
         <f>$I7-$AV7-$AZ7-$BD7</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="BI5" s="9">
         <f>$AA7</f>
@@ -1951,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:79" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:81" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
         <v>22</v>
       </c>
@@ -2030,7 +2083,9 @@
         <v>19</v>
       </c>
       <c r="AP6" s="10"/>
-      <c r="AQ6" s="9"/>
+      <c r="AQ6" s="80" t="s">
+        <v>70</v>
+      </c>
       <c r="AR6" s="9" t="s">
         <v>40</v>
       </c>
@@ -2127,7 +2182,7 @@
       <c r="BZ6" s="40"/>
       <c r="CA6" s="40"/>
     </row>
-    <row r="7" spans="1:79" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:81" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="50"/>
       <c r="B7" s="51"/>
       <c r="C7" s="42">
@@ -2147,7 +2202,7 @@
       <c r="H7" s="44"/>
       <c r="I7" s="42">
         <f>'Conversion Cheatsheet'!$B$5*I5 + 'Conversion Cheatsheet'!$D$5*J5</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J7" s="44"/>
       <c r="K7" s="17"/>
@@ -2223,7 +2278,9 @@
       <c r="AP7" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="AQ7" s="9"/>
+      <c r="AQ7" s="9">
+        <v>0</v>
+      </c>
       <c r="AR7" s="16" t="s">
         <v>44</v>
       </c>
@@ -2368,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:79" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:81" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="70" t="s">
         <v>23</v>
       </c>
@@ -2390,7 +2447,7 @@
       <c r="H8" s="47"/>
       <c r="I8" s="45">
         <f>I7*'Conversion Cheatsheet'!$K$5</f>
-        <v>0</v>
+        <v>960</v>
       </c>
       <c r="J8" s="47"/>
       <c r="K8" s="20"/>
@@ -2465,7 +2522,7 @@
       </c>
       <c r="AP8" s="20">
         <f>SUM(C8:AO8)</f>
-        <v>0</v>
+        <v>960</v>
       </c>
       <c r="AQ8" s="9"/>
       <c r="AS8" s="22"/>
@@ -2487,7 +2544,7 @@
       <c r="BO8" s="40"/>
       <c r="BP8" s="40"/>
     </row>
-    <row r="9" spans="1:79" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:81" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="54" t="s">
         <v>21</v>
       </c>
@@ -2567,7 +2624,7 @@
       </c>
       <c r="AQ9" s="9"/>
     </row>
-    <row r="10" spans="1:79" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:81" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="56"/>
       <c r="B10" s="57"/>
       <c r="C10" s="61">
@@ -2587,7 +2644,7 @@
       <c r="H10" s="61"/>
       <c r="I10" s="61">
         <f>$I7-$AV7-$AZ7-$BD7-$BH7</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J10" s="61"/>
       <c r="K10" s="15"/>
@@ -2662,7 +2719,7 @@
       </c>
       <c r="AQ10" s="9"/>
     </row>
-    <row r="11" spans="1:79" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:81" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="27"/>
@@ -2705,7 +2762,7 @@
       <c r="AN11" s="28"/>
       <c r="AO11" s="28"/>
     </row>
-    <row r="12" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="72" t="s">
@@ -2841,7 +2898,7 @@
       <c r="BZ12" s="41"/>
       <c r="CA12" s="41"/>
     </row>
-    <row r="13" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="12" t="s">
@@ -3045,7 +3102,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" s="62">
         <f>$A4+1</f>
         <v>2</v>
@@ -3066,22 +3123,30 @@
       <c r="M14" s="66"/>
       <c r="N14" s="64"/>
       <c r="O14" s="64"/>
-      <c r="P14" s="64"/>
+      <c r="P14" s="64">
+        <v>3</v>
+      </c>
       <c r="Q14" s="64"/>
       <c r="R14" s="64"/>
       <c r="S14" s="64"/>
       <c r="T14" s="64"/>
-      <c r="U14" s="64"/>
+      <c r="U14" s="64">
+        <v>2</v>
+      </c>
       <c r="V14" s="64"/>
       <c r="W14" s="64"/>
       <c r="X14" s="64"/>
       <c r="Y14" s="64"/>
-      <c r="Z14" s="64"/>
+      <c r="Z14" s="64">
+        <v>4</v>
+      </c>
       <c r="AA14" s="64"/>
       <c r="AB14" s="64"/>
       <c r="AC14" s="64"/>
       <c r="AD14" s="64"/>
-      <c r="AE14" s="64"/>
+      <c r="AE14" s="64">
+        <v>7</v>
+      </c>
       <c r="AF14" s="30"/>
       <c r="AG14" s="64"/>
       <c r="AH14" s="64"/>
@@ -3103,7 +3168,7 @@
       <c r="AU14" s="41"/>
       <c r="AV14" s="9">
         <f>FLOOR($P14/'Conversion Cheatsheet'!$E$8,1)*IF(ISBLANK($L14),2,1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW14" s="41">
         <f>FLOOR(MIN($R14/'Conversion Cheatsheet'!$B$9,$S14/'Conversion Cheatsheet'!$C$9,$T14/'Conversion Cheatsheet'!$D$9),1)*IF(ISBLANK($Q14),2,1)</f>
@@ -3113,7 +3178,7 @@
       <c r="AY14" s="41"/>
       <c r="AZ14" s="9">
         <f>FLOOR($U14/'Conversion Cheatsheet'!$E$9,1)*IF(ISBLANK($Q14),2,1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA14" s="41">
         <f>FLOOR(MIN($W14/'Conversion Cheatsheet'!$B$10,$Y14/'Conversion Cheatsheet'!$D$10),1)*IF(ISBLANK($V14),2,1)</f>
@@ -3123,7 +3188,7 @@
       <c r="BC14" s="41"/>
       <c r="BD14" s="9">
         <f>FLOOR($Z14/'Conversion Cheatsheet'!$E$9,1)*IF(ISBLANK($V14),2,1)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BE14" s="41">
         <f>FLOOR(MIN($AB14/'Conversion Cheatsheet'!$B$11,$AC14/'Conversion Cheatsheet'!$C$11,$AD14/'Conversion Cheatsheet'!$D$11),1)*IF(ISBLANK($AA14),2,1)</f>
@@ -3133,7 +3198,7 @@
       <c r="BG14" s="41"/>
       <c r="BH14" s="9">
         <f>FLOOR($AE14/'Conversion Cheatsheet'!$E$11,1)*IF(ISBLANK($AA14),2,1)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="BI14" s="9">
         <f>$AG14</f>
@@ -3191,7 +3256,7 @@
       <c r="BZ14" s="41"/>
       <c r="CA14" s="41"/>
     </row>
-    <row r="15" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" s="63"/>
       <c r="B15" s="14" t="s">
         <v>6</v>
@@ -3252,7 +3317,7 @@
       </c>
       <c r="AV15" s="16">
         <f>$I17+$I10</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="AW15" s="16">
         <f>$C17+$C10-$AS17</f>
@@ -3268,7 +3333,7 @@
       </c>
       <c r="AZ15" s="16">
         <f>$I17+$I10-$AV17</f>
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="BA15" s="16">
         <f>$C17+$C10-$AS17-$AW17</f>
@@ -3284,7 +3349,7 @@
       </c>
       <c r="BD15" s="16">
         <f>$I17+$I10-$AV17-$AZ17</f>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="BE15" s="16">
         <f>$C17+$C10-$AS17-$AW17-$BA17</f>
@@ -3300,31 +3365,31 @@
       </c>
       <c r="BH15" s="16">
         <f>$I17+$I10-$AV17-$AZ17-$BD17</f>
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="BI15" s="9">
         <f>$AA10+$AA17</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="BJ15" s="9">
         <f>$Q17+$Q10</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BK15" s="9">
         <f>$L17+$L10</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BL15" s="9">
         <f>$V17+$V10</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BM15" s="16">
         <f>$AA17+$AA10-$BI17</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="BN15" s="9">
         <f>$V17+$V10-$BL17</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BO15" s="9">
         <f>$AH17+$AH10</f>
@@ -3379,7 +3444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:79" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:81" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
         <v>22</v>
       </c>
@@ -3458,7 +3523,9 @@
         <v>19</v>
       </c>
       <c r="AP16" s="10"/>
-      <c r="AQ16" s="9"/>
+      <c r="AQ16" s="80" t="s">
+        <v>70</v>
+      </c>
       <c r="AR16" s="9" t="s">
         <v>40</v>
       </c>
@@ -3470,7 +3537,7 @@
       <c r="AU16" s="40"/>
       <c r="AV16" s="16">
         <f>FLOOR(MIN(AV14*'Conversion Cheatsheet'!$E$8,AV15)/'Conversion Cheatsheet'!$E$8,1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW16" s="40">
         <f>MIN(AW14,FLOOR(MIN(AW15/'Conversion Cheatsheet'!$B$9,AX15/'Conversion Cheatsheet'!$C$9,AY15/'Conversion Cheatsheet'!$D$9),1))</f>
@@ -3480,7 +3547,7 @@
       <c r="AY16" s="40"/>
       <c r="AZ16" s="16">
         <f>FLOOR(MIN(AZ14*'Conversion Cheatsheet'!$E$9,AZ15)/'Conversion Cheatsheet'!$E$9,1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA16" s="40">
         <f>MIN(BA14,FLOOR(MIN(BA15/'Conversion Cheatsheet'!$B$10,BC15/'Conversion Cheatsheet'!$D$10),1))</f>
@@ -3490,7 +3557,7 @@
       <c r="BC16" s="40"/>
       <c r="BD16" s="16">
         <f>FLOOR(MIN(BD14*'Conversion Cheatsheet'!$E$10,BD15)/'Conversion Cheatsheet'!$E$10,1)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BE16" s="40">
         <f>MIN(BE14,FLOOR(MIN(BE15/'Conversion Cheatsheet'!$B$11,BF15/'Conversion Cheatsheet'!$C$11,BG15/'Conversion Cheatsheet'!$D$11),1))</f>
@@ -3500,7 +3567,7 @@
       <c r="BG16" s="40"/>
       <c r="BH16" s="16">
         <f>FLOOR(MIN(BH14*'Conversion Cheatsheet'!$E$11,BH15)/'Conversion Cheatsheet'!$E$11,1)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="BI16" s="16">
         <f t="shared" ref="BI16:BN16" si="3">MIN(BI14,BI15)</f>
@@ -3581,7 +3648,7 @@
       <c r="K17" s="17"/>
       <c r="L17" s="42">
         <f>$AS16+$AV16</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M17" s="43"/>
       <c r="N17" s="43"/>
@@ -3589,7 +3656,7 @@
       <c r="P17" s="44"/>
       <c r="Q17" s="42">
         <f>$AW16+$AZ16</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R17" s="43"/>
       <c r="S17" s="43"/>
@@ -3597,7 +3664,7 @@
       <c r="U17" s="44"/>
       <c r="V17" s="42">
         <f>$BA16+$BD16</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W17" s="43"/>
       <c r="X17" s="43"/>
@@ -3605,7 +3672,7 @@
       <c r="Z17" s="44"/>
       <c r="AA17" s="42">
         <f>$BE16+$BH16</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AB17" s="43"/>
       <c r="AC17" s="43"/>
@@ -3651,7 +3718,9 @@
       <c r="AP17" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="AQ17" s="9"/>
+      <c r="AQ17" s="9">
+        <v>1</v>
+      </c>
       <c r="AR17" s="16" t="s">
         <v>44</v>
       </c>
@@ -3669,7 +3738,7 @@
       </c>
       <c r="AV17" s="16">
         <f>AV16*'Conversion Cheatsheet'!$E$8</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AW17" s="16">
         <f>'Conversion Cheatsheet'!$B$9*AW16</f>
@@ -3685,7 +3754,7 @@
       </c>
       <c r="AZ17" s="16">
         <f>AZ16*'Conversion Cheatsheet'!$E$9</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BA17" s="16">
         <f>'Conversion Cheatsheet'!$B$10*BA16</f>
@@ -3701,7 +3770,7 @@
       </c>
       <c r="BD17" s="16">
         <f>BD16*'Conversion Cheatsheet'!$E$10</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="BE17" s="16">
         <f>'Conversion Cheatsheet'!$B$11*BE16</f>
@@ -3717,7 +3786,7 @@
       </c>
       <c r="BH17" s="16">
         <f>BH16*'Conversion Cheatsheet'!$E$11</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="BI17" s="16">
         <f t="shared" ref="BI17:BN17" si="7">BI16</f>
@@ -3824,7 +3893,7 @@
       <c r="K18" s="20"/>
       <c r="L18" s="45">
         <f>$L17*'Conversion Cheatsheet'!$K$7</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="M18" s="46"/>
       <c r="N18" s="46"/>
@@ -3832,7 +3901,7 @@
       <c r="P18" s="47"/>
       <c r="Q18" s="45">
         <f>$Q17*'Conversion Cheatsheet'!$K$8</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R18" s="46"/>
       <c r="S18" s="46"/>
@@ -3840,7 +3909,7 @@
       <c r="U18" s="47"/>
       <c r="V18" s="45">
         <f>$V17*'Conversion Cheatsheet'!$K$9</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="W18" s="46"/>
       <c r="X18" s="46"/>
@@ -3848,7 +3917,7 @@
       <c r="Z18" s="47"/>
       <c r="AA18" s="45">
         <f>$AA17*'Conversion Cheatsheet'!$K$10</f>
-        <v>0</v>
+        <v>840</v>
       </c>
       <c r="AB18" s="46"/>
       <c r="AC18" s="46"/>
@@ -3893,7 +3962,7 @@
       </c>
       <c r="AP18" s="20">
         <f>SUM(C18:AO18)</f>
-        <v>0</v>
+        <v>1280</v>
       </c>
       <c r="AQ18" s="9"/>
       <c r="AS18" s="40"/>
@@ -4000,13 +4069,13 @@
       <c r="H20" s="61"/>
       <c r="I20" s="61">
         <f>$I17+$I10-$AV17-$AZ17-$BD17-$BH17</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="J20" s="61"/>
       <c r="K20" s="15"/>
       <c r="L20" s="61">
         <f>$L17+$L10-$BK17</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M20" s="61"/>
       <c r="N20" s="61"/>
@@ -4014,7 +4083,7 @@
       <c r="P20" s="61"/>
       <c r="Q20" s="61">
         <f>$Q17+$Q10-$BJ17</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R20" s="61"/>
       <c r="S20" s="61"/>
@@ -4022,7 +4091,7 @@
       <c r="U20" s="61"/>
       <c r="V20" s="61">
         <f>$V17+$V10-$BL17-$BN17</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W20" s="61"/>
       <c r="X20" s="61"/>
@@ -4030,7 +4099,7 @@
       <c r="Z20" s="61"/>
       <c r="AA20" s="61">
         <f>$AA17+$AA10-$BI17-$BQ17-$BR17</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AB20" s="61"/>
       <c r="AC20" s="61"/>
@@ -4496,12 +4565,24 @@
       <c r="AD24" s="64"/>
       <c r="AE24" s="64"/>
       <c r="AF24" s="30"/>
-      <c r="AG24" s="64"/>
-      <c r="AH24" s="64"/>
-      <c r="AI24" s="64"/>
-      <c r="AJ24" s="64"/>
-      <c r="AK24" s="64"/>
-      <c r="AL24" s="64"/>
+      <c r="AG24" s="64">
+        <v>3</v>
+      </c>
+      <c r="AH24" s="64">
+        <v>1</v>
+      </c>
+      <c r="AI24" s="64">
+        <v>1</v>
+      </c>
+      <c r="AJ24" s="64">
+        <v>1</v>
+      </c>
+      <c r="AK24" s="64">
+        <v>4</v>
+      </c>
+      <c r="AL24" s="64">
+        <v>1</v>
+      </c>
       <c r="AM24" s="75"/>
       <c r="AN24" s="76"/>
       <c r="AO24" s="10"/>
@@ -4550,31 +4631,31 @@
       </c>
       <c r="BI24" s="9">
         <f>$AG24</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BJ24" s="9">
         <f>IF(OR($AH24=0,ISBLANK($AH24)),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK24" s="9">
         <f>IF(OR($AI24=0,ISBLANK($AI24)),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL24" s="9">
         <f>IF(OR($AJ24=0,ISBLANK($AJ24)),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM24" s="9">
         <f>$AK24</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BN24" s="9">
         <f>IF(OR($AL24=0,ISBLANK($AL24)),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO24" s="41">
         <f>IF(AND($AH24+$AH20&gt;0,$AI24+$AI20&gt;0),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP24" s="41"/>
       <c r="BQ24" s="9">
@@ -4583,7 +4664,7 @@
       </c>
       <c r="BR24" s="41">
         <f>IF(AND(AK24='Conversion Cheatsheet'!$B$15,$BN26=1),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS24" s="41">
         <f>IF(AND(AM24&gt;='Conversion Cheatsheet'!$B$14,$BN26&lt;1),1,0)</f>
@@ -4598,7 +4679,7 @@
       <c r="BW24" s="41"/>
       <c r="BX24" s="41">
         <f>IF(AND($AG27+AG20&gt;='Conversion Cheatsheet'!$B$19,$AJ27+AJ20&gt;='Conversion Cheatsheet'!$C$19,$AK27+AK20&gt;='Conversion Cheatsheet'!$E$19,$AM27+AM20&gt;='Conversion Cheatsheet'!$H$19),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY24" s="41"/>
       <c r="BZ24" s="41"/>
@@ -4665,7 +4746,7 @@
       </c>
       <c r="AV25" s="16">
         <f>$I27+$I20</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="AW25" s="16">
         <f>$C27+$C20-$AS27</f>
@@ -4681,7 +4762,7 @@
       </c>
       <c r="AZ25" s="16">
         <f>$I27+$I20-$AV27</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BA25" s="16">
         <f>$C27+$C20-$AS27-$AW27</f>
@@ -4697,7 +4778,7 @@
       </c>
       <c r="BD25" s="16">
         <f>$I27+$I20-$AV27-$AZ27</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BE25" s="16">
         <f>$C27+$C20-$AS27-$AW27-$BA27</f>
@@ -4713,63 +4794,63 @@
       </c>
       <c r="BH25" s="16">
         <f>$I27+$I20-$AV27-$AZ27-$BD27</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BI25" s="9">
         <f>$AA20+$AA27</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="BJ25" s="9">
         <f>$Q27+$Q20</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BK25" s="9">
         <f>$L27+$L20</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BL25" s="9">
         <f>$V27+$V20</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BM25" s="16">
         <f>$AA27+$AA20-$BI27</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="BN25" s="9">
         <f>$V27+$V20-$BL27</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BO25" s="9">
         <f>$AH27+$AH20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP25" s="9">
         <f>$AI27+$AI20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ25" s="9">
         <f>BM26</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BR25" s="9">
         <f>BM26</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BS25" s="9">
         <f>BN26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT25" s="9">
         <f>$AG20+$BI26</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BU25" s="9">
         <f>$BO26+$AK20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BV25" s="9">
         <f>$BL26+$AJ20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW25" s="9">
         <f>$BQ26+$AM20</f>
@@ -4777,19 +4858,19 @@
       </c>
       <c r="BX25" s="9">
         <f>$AG20+$BI26</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BY25" s="9">
         <f>$BO26+$AK20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ25" s="9">
         <f>$BL26+$AJ20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA25" s="9">
         <f>$BR26+$AO20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:79" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -4871,7 +4952,9 @@
         <v>19</v>
       </c>
       <c r="AP26" s="10"/>
-      <c r="AQ26" s="9"/>
+      <c r="AQ26" s="80" t="s">
+        <v>70</v>
+      </c>
       <c r="AR26" s="9" t="s">
         <v>40</v>
       </c>
@@ -4917,31 +5000,31 @@
       </c>
       <c r="BI26" s="16">
         <f t="shared" ref="BI26:BN26" si="8">MIN(BI24,BI25)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BJ26" s="16">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK26" s="16">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL26" s="16">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM26" s="16">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BN26" s="16">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO26" s="41">
         <f>IF(AND($BO24&gt;0,$BO25&gt;0,$BP25&gt;0),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP26" s="41"/>
       <c r="BQ26" s="16">
@@ -4950,7 +5033,7 @@
       </c>
       <c r="BR26" s="40">
         <f>IF(AND(BR24&gt;0,BR25='Conversion Cheatsheet'!$B$15,BS25='Conversion Cheatsheet'!$C$15),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS26" s="40"/>
       <c r="BT26" s="40">
@@ -4962,7 +5045,7 @@
       <c r="BW26" s="40"/>
       <c r="BX26" s="40">
         <f>BX24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY26" s="40"/>
       <c r="BZ26" s="40"/>
@@ -5027,23 +5110,23 @@
       <c r="AF27" s="17"/>
       <c r="AG27" s="18">
         <f>BI26</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH27" s="18">
         <f t="shared" ref="AH27" si="9">BJ26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI27" s="18">
         <f t="shared" ref="AI27" si="10">BK26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ27" s="18">
         <f t="shared" ref="AJ27" si="11">BL26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK27" s="18">
         <f>BO26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL27" s="18">
         <f>BQ26</f>
@@ -5051,7 +5134,7 @@
       </c>
       <c r="AM27" s="18">
         <f>BR26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN27" s="17">
         <f>BT26</f>
@@ -5059,12 +5142,14 @@
       </c>
       <c r="AO27" s="17">
         <f>BX26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP27" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="AQ27" s="9"/>
+      <c r="AQ27" s="9">
+        <v>1</v>
+      </c>
       <c r="AR27" s="16" t="s">
         <v>44</v>
       </c>
@@ -5134,35 +5219,35 @@
       </c>
       <c r="BI27" s="16">
         <f t="shared" ref="BI27:BN27" si="12">BI26</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BJ27" s="16">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK27" s="16">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL27" s="16">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM27" s="16">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BN27" s="16">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO27" s="16">
         <f>BO26*BO25</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP27" s="16">
         <f>BO26*BP25</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ27" s="16">
         <f>BQ26</f>
@@ -5170,11 +5255,11 @@
       </c>
       <c r="BR27" s="16">
         <f>BR26*BR25</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BS27" s="16">
         <f>BR26*BS25</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT27" s="16">
         <f>'Conversion Cheatsheet'!$B$18*$BT26</f>
@@ -5194,19 +5279,19 @@
       </c>
       <c r="BX27" s="16">
         <f>'Conversion Cheatsheet'!$B$19*$BX26</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BY27" s="16">
         <f>'Conversion Cheatsheet'!$C$19*$BX26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ27" s="16">
         <f>'Conversion Cheatsheet'!$E$19*$BX26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA27" s="16">
         <f>'Conversion Cheatsheet'!$H$19*$BX26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:79" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -5270,19 +5355,19 @@
       <c r="AF28" s="20"/>
       <c r="AG28" s="21">
         <f>AG27*'Conversion Cheatsheet'!$K$12</f>
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="AH28" s="21">
         <f>AH27*'Conversion Cheatsheet'!$K$13</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="AI28" s="21">
         <f>AI27*'Conversion Cheatsheet'!$K$14</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="AJ28" s="21">
         <f>AJ27*'Conversion Cheatsheet'!$K$15</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="AK28" s="21">
         <f>AK27*'Conversion Cheatsheet'!$K$16</f>
@@ -5294,7 +5379,7 @@
       </c>
       <c r="AM28" s="21">
         <f>AM27*'Conversion Cheatsheet'!$K$18</f>
-        <v>0</v>
+        <v>420</v>
       </c>
       <c r="AN28" s="21">
         <f>AN27*'Conversion Cheatsheet'!$K$20</f>
@@ -5302,11 +5387,11 @@
       </c>
       <c r="AO28" s="21">
         <f>AO27*'Conversion Cheatsheet'!$K$21</f>
-        <v>0</v>
+        <v>1024</v>
       </c>
       <c r="AP28" s="20">
         <f>SUM(C28:AO28)</f>
-        <v>0</v>
+        <v>1984</v>
       </c>
       <c r="AQ28" s="9"/>
       <c r="AS28" s="40"/>
@@ -5413,13 +5498,13 @@
       <c r="H30" s="61"/>
       <c r="I30" s="61">
         <f>$I27+$I20-$AV27-$AZ27-$BD27-$BH27</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="J30" s="61"/>
       <c r="K30" s="15"/>
       <c r="L30" s="61">
         <f>$L27+$L20-$BK27</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M30" s="61"/>
       <c r="N30" s="61"/>
@@ -5427,7 +5512,7 @@
       <c r="P30" s="61"/>
       <c r="Q30" s="61">
         <f>$Q27+$Q20-$BJ27</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R30" s="61"/>
       <c r="S30" s="61"/>
@@ -5435,7 +5520,7 @@
       <c r="U30" s="61"/>
       <c r="V30" s="61">
         <f>$V27+$V20-$BL27-$BN27</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W30" s="61"/>
       <c r="X30" s="61"/>
@@ -5443,7 +5528,7 @@
       <c r="Z30" s="61"/>
       <c r="AA30" s="61">
         <f>$AA27+$AA20-$BI27-$BQ27-$BR27</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AB30" s="61"/>
       <c r="AC30" s="61"/>
@@ -5484,7 +5569,7 @@
       </c>
       <c r="AO30" s="15">
         <f>$BX26+$AO20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ30" s="9"/>
     </row>
@@ -5532,7 +5617,9 @@
       <c r="AO31" s="28"/>
     </row>
     <row r="32" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
+      <c r="A32" s="10">
+        <v>1</v>
+      </c>
       <c r="B32" s="10"/>
       <c r="C32" s="72" t="s">
         <v>0</v>
@@ -6078,7 +6165,7 @@
       </c>
       <c r="AV35" s="16">
         <f>$I37+$I30</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="AW35" s="16">
         <f>$C37+$C30-$AS37</f>
@@ -6094,7 +6181,7 @@
       </c>
       <c r="AZ35" s="16">
         <f>$I37+$I30-$AV37</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BA35" s="16">
         <f>$C37+$C30-$AS37-$AW37</f>
@@ -6110,7 +6197,7 @@
       </c>
       <c r="BD35" s="16">
         <f>$I37+$I30-$AV37-$AZ37</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BE35" s="16">
         <f>$C37+$C30-$AS37-$AW37-$BA37</f>
@@ -6126,31 +6213,31 @@
       </c>
       <c r="BH35" s="16">
         <f>$I37+$I30-$AV37-$AZ37-$BD37</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BI35" s="9">
         <f>$AA30+$AA37</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BJ35" s="9">
         <f>$Q37+$Q30</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK35" s="9">
         <f>$L37+$L30</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL35" s="9">
         <f>$V37+$V30</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BM35" s="16">
         <f>$AA37+$AA30-$BI37</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BN35" s="9">
         <f>$V37+$V30-$BL37</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BO35" s="9">
         <f>$AH37+$AH30</f>
@@ -6202,7 +6289,7 @@
       </c>
       <c r="CA35" s="9">
         <f>$BR36+$AO30</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:79" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -6284,7 +6371,9 @@
         <v>19</v>
       </c>
       <c r="AP36" s="10"/>
-      <c r="AQ36" s="9"/>
+      <c r="AQ36" s="80" t="s">
+        <v>70</v>
+      </c>
       <c r="AR36" s="9" t="s">
         <v>40</v>
       </c>
@@ -6826,13 +6915,13 @@
       <c r="H40" s="61"/>
       <c r="I40" s="61">
         <f>$I37+$I30-$AV37-$AZ37-$BD37-$BH37</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="J40" s="61"/>
       <c r="K40" s="15"/>
       <c r="L40" s="61">
         <f>$L37+$L30-$BK37</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M40" s="61"/>
       <c r="N40" s="61"/>
@@ -6840,7 +6929,7 @@
       <c r="P40" s="61"/>
       <c r="Q40" s="61">
         <f>$Q37+$Q30-$BJ37</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R40" s="61"/>
       <c r="S40" s="61"/>
@@ -6848,7 +6937,7 @@
       <c r="U40" s="61"/>
       <c r="V40" s="61">
         <f>$V37+$V30-$BL37-$BN37</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W40" s="61"/>
       <c r="X40" s="61"/>
@@ -6856,7 +6945,7 @@
       <c r="Z40" s="61"/>
       <c r="AA40" s="61">
         <f>$AA37+$AA30-$BI37-$BQ37-$BR37</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AB40" s="61"/>
       <c r="AC40" s="61"/>
@@ -6897,7 +6986,7 @@
       </c>
       <c r="AO40" s="15">
         <f>$BX36+$AO30</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ40" s="9"/>
     </row>
@@ -6945,7 +7034,9 @@
       <c r="AO41" s="28"/>
     </row>
     <row r="42" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
+      <c r="A42" s="10">
+        <v>1</v>
+      </c>
       <c r="B42" s="10"/>
       <c r="C42" s="72" t="s">
         <v>0</v>
@@ -7491,7 +7582,7 @@
       </c>
       <c r="AV45" s="16">
         <f>$I47+$I40</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="AW45" s="16">
         <f>$C47+$C40-$AS47</f>
@@ -7507,7 +7598,7 @@
       </c>
       <c r="AZ45" s="16">
         <f>$I47+$I40-$AV47</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BA45" s="16">
         <f>$C47+$C40-$AS47-$AW47</f>
@@ -7523,7 +7614,7 @@
       </c>
       <c r="BD45" s="16">
         <f>$I47+$I40-$AV47-$AZ47</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BE45" s="16">
         <f>$C47+$C40-$AS47-$AW47-$BA47</f>
@@ -7539,31 +7630,31 @@
       </c>
       <c r="BH45" s="16">
         <f>$I47+$I40-$AV47-$AZ47-$BD47</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BI45" s="9">
         <f>$AA40+$AA47</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BJ45" s="9">
         <f>$Q47+$Q40</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK45" s="9">
         <f>$L47+$L40</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL45" s="9">
         <f>$V47+$V40</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BM45" s="16">
         <f>$AA47+$AA40-$BI47</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BN45" s="9">
         <f>$V47+$V40-$BL47</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BO45" s="9">
         <f>$AH47+$AH40</f>
@@ -7615,7 +7706,7 @@
       </c>
       <c r="CA45" s="9">
         <f>$BR46+$AO40</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:79" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -7697,7 +7788,9 @@
         <v>19</v>
       </c>
       <c r="AP46" s="10"/>
-      <c r="AQ46" s="9"/>
+      <c r="AQ46" s="80" t="s">
+        <v>70</v>
+      </c>
       <c r="AR46" s="9" t="s">
         <v>40</v>
       </c>
@@ -8239,13 +8332,13 @@
       <c r="H50" s="61"/>
       <c r="I50" s="61">
         <f>$I47+$I40-$AV47-$AZ47-$BD47-$BH47</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="J50" s="61"/>
       <c r="K50" s="15"/>
       <c r="L50" s="61">
         <f>$L47+$L40-$BK47</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M50" s="61"/>
       <c r="N50" s="61"/>
@@ -8253,7 +8346,7 @@
       <c r="P50" s="61"/>
       <c r="Q50" s="61">
         <f>$Q47+$Q40-$BJ47</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R50" s="61"/>
       <c r="S50" s="61"/>
@@ -8261,7 +8354,7 @@
       <c r="U50" s="61"/>
       <c r="V50" s="61">
         <f>$V47+$V40-$BL47-$BN47</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W50" s="61"/>
       <c r="X50" s="61"/>
@@ -8269,7 +8362,7 @@
       <c r="Z50" s="61"/>
       <c r="AA50" s="61">
         <f>$AA47+$AA40-$BI47-$BQ47-$BR47</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AB50" s="61"/>
       <c r="AC50" s="61"/>
@@ -8310,7 +8403,7 @@
       </c>
       <c r="AO50" s="15">
         <f>$BX46+$AO40</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ50" s="9"/>
     </row>
@@ -8358,7 +8451,9 @@
       <c r="AO51" s="28"/>
     </row>
     <row r="52" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A52" s="10"/>
+      <c r="A52" s="10">
+        <v>1</v>
+      </c>
       <c r="B52" s="10"/>
       <c r="C52" s="72" t="s">
         <v>0</v>
@@ -8904,7 +8999,7 @@
       </c>
       <c r="AV55" s="16">
         <f>$I57+$I50</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="AW55" s="16">
         <f>$C57+$C50-$AS57</f>
@@ -8920,7 +9015,7 @@
       </c>
       <c r="AZ55" s="16">
         <f>$I57+$I50-$AV57</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BA55" s="16">
         <f>$C57+$C50-$AS57-$AW57</f>
@@ -8936,7 +9031,7 @@
       </c>
       <c r="BD55" s="16">
         <f>$I57+$I50-$AV57-$AZ57</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BE55" s="16">
         <f>$C57+$C50-$AS57-$AW57-$BA57</f>
@@ -8952,31 +9047,31 @@
       </c>
       <c r="BH55" s="16">
         <f>$I57+$I50-$AV57-$AZ57-$BD57</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BI55" s="9">
         <f>$AA50+$AA57</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BJ55" s="9">
         <f>$Q57+$Q50</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK55" s="9">
         <f>$L57+$L50</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL55" s="9">
         <f>$V57+$V50</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BM55" s="16">
         <f>$AA57+$AA50-$BI57</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BN55" s="9">
         <f>$V57+$V50-$BL57</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BO55" s="9">
         <f>$AH57+$AH50</f>
@@ -9028,7 +9123,7 @@
       </c>
       <c r="CA55" s="9">
         <f>$BR56+$AO50</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:79" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -9110,7 +9205,9 @@
         <v>19</v>
       </c>
       <c r="AP56" s="10"/>
-      <c r="AQ56" s="9"/>
+      <c r="AQ56" s="80" t="s">
+        <v>70</v>
+      </c>
       <c r="AR56" s="9" t="s">
         <v>40</v>
       </c>
@@ -9652,13 +9749,13 @@
       <c r="H60" s="61"/>
       <c r="I60" s="61">
         <f>$I57+$I50-$AV57-$AZ57-$BD57-$BH57</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="J60" s="61"/>
       <c r="K60" s="15"/>
       <c r="L60" s="61">
         <f>$L57+$L50-$BK57</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M60" s="61"/>
       <c r="N60" s="61"/>
@@ -9666,7 +9763,7 @@
       <c r="P60" s="61"/>
       <c r="Q60" s="61">
         <f>$Q57+$Q50-$BJ57</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R60" s="61"/>
       <c r="S60" s="61"/>
@@ -9674,7 +9771,7 @@
       <c r="U60" s="61"/>
       <c r="V60" s="61">
         <f>$V57+$V50-$BL57-$BN57</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W60" s="61"/>
       <c r="X60" s="61"/>
@@ -9682,7 +9779,7 @@
       <c r="Z60" s="61"/>
       <c r="AA60" s="61">
         <f>$AA57+$AA50-$BI57-$BQ57-$BR57</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AB60" s="61"/>
       <c r="AC60" s="61"/>
@@ -9723,7 +9820,7 @@
       </c>
       <c r="AO60" s="15">
         <f>$BX56+$AO50</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ60" s="9"/>
     </row>
@@ -9771,7 +9868,9 @@
       <c r="AO61" s="28"/>
     </row>
     <row r="62" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A62" s="10"/>
+      <c r="A62" s="10">
+        <v>1</v>
+      </c>
       <c r="B62" s="10"/>
       <c r="C62" s="72" t="s">
         <v>0</v>
@@ -10317,7 +10416,7 @@
       </c>
       <c r="AV65" s="16">
         <f>$I67+$I60</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="AW65" s="16">
         <f>$C67+$C60-$AS67</f>
@@ -10333,7 +10432,7 @@
       </c>
       <c r="AZ65" s="16">
         <f>$I67+$I60-$AV67</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BA65" s="16">
         <f>$C67+$C60-$AS67-$AW67</f>
@@ -10349,7 +10448,7 @@
       </c>
       <c r="BD65" s="16">
         <f>$I67+$I60-$AV67-$AZ67</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BE65" s="16">
         <f>$C67+$C60-$AS67-$AW67-$BA67</f>
@@ -10365,31 +10464,31 @@
       </c>
       <c r="BH65" s="16">
         <f>$I67+$I60-$AV67-$AZ67-$BD67</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BI65" s="9">
         <f>$AA60+$AA67</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BJ65" s="9">
         <f>$Q67+$Q60</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK65" s="9">
         <f>$L67+$L60</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL65" s="9">
         <f>$V67+$V60</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BM65" s="16">
         <f>$AA67+$AA60-$BI67</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BN65" s="9">
         <f>$V67+$V60-$BL67</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BO65" s="9">
         <f>$AH67+$AH60</f>
@@ -10441,7 +10540,7 @@
       </c>
       <c r="CA65" s="9">
         <f>$BR66+$AO60</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:79" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -10523,7 +10622,9 @@
         <v>19</v>
       </c>
       <c r="AP66" s="10"/>
-      <c r="AQ66" s="9"/>
+      <c r="AQ66" s="80" t="s">
+        <v>70</v>
+      </c>
       <c r="AR66" s="9" t="s">
         <v>40</v>
       </c>
@@ -11065,13 +11166,13 @@
       <c r="H70" s="61"/>
       <c r="I70" s="61">
         <f>$I67+$I60-$AV67-$AZ67-$BD67-$BH67</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="J70" s="61"/>
       <c r="K70" s="15"/>
       <c r="L70" s="61">
         <f>$L67+$L60-$BK67</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M70" s="61"/>
       <c r="N70" s="61"/>
@@ -11079,7 +11180,7 @@
       <c r="P70" s="61"/>
       <c r="Q70" s="61">
         <f>$Q67+$Q60-$BJ67</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R70" s="61"/>
       <c r="S70" s="61"/>
@@ -11087,7 +11188,7 @@
       <c r="U70" s="61"/>
       <c r="V70" s="61">
         <f>$V67+$V60-$BL67-$BN67</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W70" s="61"/>
       <c r="X70" s="61"/>
@@ -11095,7 +11196,7 @@
       <c r="Z70" s="61"/>
       <c r="AA70" s="61">
         <f>$AA67+$AA60-$BI67-$BQ67-$BR67</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AB70" s="61"/>
       <c r="AC70" s="61"/>
@@ -11136,7 +11237,7 @@
       </c>
       <c r="AO70" s="15">
         <f>$BX66+$AO60</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ70" s="9"/>
     </row>
@@ -11184,7 +11285,9 @@
       <c r="AO71" s="28"/>
     </row>
     <row r="72" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A72" s="10"/>
+      <c r="A72" s="10">
+        <v>1</v>
+      </c>
       <c r="B72" s="10"/>
       <c r="C72" s="72" t="s">
         <v>0</v>
@@ -11730,7 +11833,7 @@
       </c>
       <c r="AV75" s="16">
         <f>$I77+$I70</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="AW75" s="16">
         <f>$C77+$C70-$AS77</f>
@@ -11746,7 +11849,7 @@
       </c>
       <c r="AZ75" s="16">
         <f>$I77+$I70-$AV77</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BA75" s="16">
         <f>$C77+$C70-$AS77-$AW77</f>
@@ -11762,7 +11865,7 @@
       </c>
       <c r="BD75" s="16">
         <f>$I77+$I70-$AV77-$AZ77</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BE75" s="16">
         <f>$C77+$C70-$AS77-$AW77-$BA77</f>
@@ -11778,31 +11881,31 @@
       </c>
       <c r="BH75" s="16">
         <f>$I77+$I70-$AV77-$AZ77-$BD77</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="BI75" s="9">
         <f>$AA70+$AA77</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BJ75" s="9">
         <f>$Q77+$Q70</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK75" s="9">
         <f>$L77+$L70</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL75" s="9">
         <f>$V77+$V70</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BM75" s="16">
         <f>$AA77+$AA70-$BI77</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BN75" s="9">
         <f>$V77+$V70-$BL77</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BO75" s="9">
         <f>$AH77+$AH70</f>
@@ -11854,7 +11957,7 @@
       </c>
       <c r="CA75" s="9">
         <f>$BR76+$AO70</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:79" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -11936,7 +12039,9 @@
         <v>19</v>
       </c>
       <c r="AP76" s="10"/>
-      <c r="AQ76" s="9"/>
+      <c r="AQ76" s="80" t="s">
+        <v>70</v>
+      </c>
       <c r="AR76" s="9" t="s">
         <v>40</v>
       </c>
@@ -12478,13 +12583,13 @@
       <c r="H80" s="61"/>
       <c r="I80" s="61">
         <f>$I77+$I70-$AV77-$AZ77-$BD77-$BH77</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="J80" s="61"/>
       <c r="K80" s="15"/>
       <c r="L80" s="61">
         <f>$L77+$L70-$BK77</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M80" s="61"/>
       <c r="N80" s="61"/>
@@ -12492,7 +12597,7 @@
       <c r="P80" s="61"/>
       <c r="Q80" s="61">
         <f>$Q77+$Q70-$BJ77</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R80" s="61"/>
       <c r="S80" s="61"/>
@@ -12500,7 +12605,7 @@
       <c r="U80" s="61"/>
       <c r="V80" s="61">
         <f>$V77+$V70-$BL77-$BN77</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W80" s="61"/>
       <c r="X80" s="61"/>
@@ -12508,7 +12613,7 @@
       <c r="Z80" s="61"/>
       <c r="AA80" s="61">
         <f>$AA77+$AA70-$BI77-$BQ77-$BR77</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AB80" s="61"/>
       <c r="AC80" s="61"/>
@@ -12549,7 +12654,7 @@
       </c>
       <c r="AO80" s="15">
         <f>$BX76+$AO70</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ80" s="9"/>
     </row>
@@ -12597,7 +12702,6 @@
       <c r="AO81" s="28"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="881">
     <mergeCell ref="AS76:AU76"/>
     <mergeCell ref="AW76:AY76"/>
@@ -13489,10 +13593,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:AB22"/>
+  <dimension ref="A1:AD22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="AD10" sqref="AD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13506,7 +13610,7 @@
     <col min="14" max="19" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>45</v>
       </c>
@@ -13543,8 +13647,14 @@
       <c r="W1" t="s">
         <v>68</v>
       </c>
+      <c r="AC1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -13614,8 +13724,16 @@
       <c r="AB2" t="s">
         <v>68</v>
       </c>
+      <c r="AC2">
+        <f>'Team Scoresheet'!AQ7</f>
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <f>'Team Scoresheet'!A2</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -13660,8 +13778,16 @@
       <c r="AB3">
         <v>1792</v>
       </c>
+      <c r="AC3">
+        <f>'Team Scoresheet'!AQ17</f>
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <f>'Team Scoresheet'!A12</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -13728,8 +13854,16 @@
         <f>$K12*3</f>
         <v>270</v>
       </c>
+      <c r="AC4">
+        <f>'Team Scoresheet'!AQ27</f>
+        <v>1</v>
+      </c>
+      <c r="AD4">
+        <f>'Team Scoresheet'!A22</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -13791,8 +13925,16 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
+      <c r="AC5">
+        <f>'Team Scoresheet'!AQ37</f>
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <f>'Team Scoresheet'!A32</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -13842,8 +13984,16 @@
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
+      <c r="AC6">
+        <f>'Team Scoresheet'!AQ47</f>
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <f>'Team Scoresheet'!A42</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -13904,8 +14054,16 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
+      <c r="AC7">
+        <f>'Team Scoresheet'!AQ57</f>
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <f>'Team Scoresheet'!A52</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -13965,8 +14123,16 @@
         <f>$K18</f>
         <v>420</v>
       </c>
+      <c r="AC8">
+        <f>'Team Scoresheet'!AQ67</f>
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <f>'Team Scoresheet'!A62</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -13993,8 +14159,16 @@
         <v>40</v>
       </c>
       <c r="L9" s="2"/>
+      <c r="AC9">
+        <f>'Team Scoresheet'!AQ77</f>
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <f>'Team Scoresheet'!A72</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -14041,7 +14215,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -14084,7 +14258,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -14121,7 +14295,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>24</v>
       </c>
@@ -14161,7 +14335,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -14185,7 +14359,7 @@
       </c>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -14226,7 +14400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>